<commit_message>
Added Boats Search test case on API level
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_ReservationBoatsSearch_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_ReservationBoatsSearch_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmoud El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8074EBA2-B5B8-4004-8AD3-3FC936B32F90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1F5FCF-641A-4689-B52F-A27ADC80878E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>TC ID/Name</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>Expected Boat Name</t>
+  </si>
+  <si>
+    <t>Country Name</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>istanbul</t>
+  </si>
+  <si>
+    <t>Motor-boat-Custom-Built---2005-refit-2017-</t>
   </si>
 </sst>
 </file>
@@ -441,59 +456,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A63622E-CB57-6443-8D5E-E59E3D20E8B5}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,23 +528,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5A4EB-72C8-0E44-91C4-D3652BB51352}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -543,7 +565,7 @@
       </c>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,7 +599,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>